<commit_message>
#3557: enabling locale functionality in non-template mode
</commit_message>
<xml_diff>
--- a/node_modules/msoffice/lib/excel/template.xlsx
+++ b/node_modules/msoffice/lib/excel/template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Syracuse\source\Syracuse\node_modules\msoffice\lib\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="13395" windowHeight="6210" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="13392" windowHeight="6216"/>
   </bookViews>
   <sheets>
     <sheet name="Sage.X3.ReservedSheet" sheetId="4" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>___dictionnary___</t>
   </si>
@@ -31,10 +36,13 @@
     <t>___documentTitle___</t>
   </si>
   <si>
+    <t>___addInDownloadLabel___</t>
+  </si>
+  <si>
+    <t>___addSupportedLocales___</t>
+  </si>
+  <si>
     <t>___datasources___</t>
-  </si>
-  <si>
-    <t>___addInDownloadLabel___</t>
   </si>
 </sst>
 </file>
@@ -178,6 +186,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -225,7 +236,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,7 +271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,38 +481,45 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -514,13 +532,13 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -551,7 +569,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>